<commit_message>
adding results for nitfi header fix
</commit_message>
<xml_diff>
--- a/Documentation/results all tests.xlsx
+++ b/Documentation/results all tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23840" windowHeight="15600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24680" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="varying ref for MC" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="37">
   <si>
     <t>a)</t>
   </si>
@@ -58,9 +58,6 @@
     <t>nb of voxels with variance explained &gt;10%</t>
   </si>
   <si>
-    <t>% of voxels with variance explained &gt;10%</t>
-  </si>
-  <si>
     <t>Total nb of voxels</t>
   </si>
   <si>
@@ -128,15 +125,22 @@
   </si>
   <si>
     <t>Pipeline_JAS (new) using MC with ref 3 (TR1 of EPI1) / no slice timing correction /  class-file itkGray edit (except for KM79) / no motion outlier removed / 5-step inplane-anat registr. / pRF-rmMain’s wSearch 3</t>
+  </si>
+  <si>
+    <t>% of good voxels with variance explained &gt;10%</t>
+  </si>
+  <si>
+    <t>nb of good voxels with variance explained &gt;10%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -324,8 +328,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -439,9 +469,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -461,9 +488,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -480,9 +504,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -498,9 +519,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -576,8 +594,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -608,6 +638,19 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -638,6 +681,19 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -969,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -988,193 +1044,193 @@
     <col min="11" max="11" width="9" style="17" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.1640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" style="25" customWidth="1"/>
-    <col min="18" max="18" width="9.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.83203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9" style="32" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="32" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="32" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.33203125" style="39" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.83203125" style="39" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9" style="39" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.1640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9" style="39" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="24" customWidth="1"/>
+    <col min="18" max="18" width="9.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.83203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" style="30" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.1640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" style="30" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.83203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" style="36" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9" style="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="20" customHeight="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="50"/>
+      <c r="H1" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+    </row>
+    <row r="2" spans="1:28" ht="78" customHeight="1">
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="63"/>
+      <c r="L2" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="58"/>
+    </row>
+    <row r="3" spans="1:28" ht="21" customHeight="1">
+      <c r="A3" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="67">
+        <v>2.0125000000000001E-2</v>
+      </c>
+      <c r="I3" s="67"/>
+      <c r="J3" s="64">
+        <v>5.8588166441834577</v>
+      </c>
+      <c r="K3" s="64"/>
+      <c r="L3" s="58">
+        <v>22936</v>
+      </c>
+      <c r="M3" s="58"/>
+    </row>
+    <row r="4" spans="1:28" ht="15" customHeight="1">
+      <c r="A4" s="58"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+    </row>
+    <row r="5" spans="1:28" ht="20" customHeight="1">
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+    </row>
+    <row r="6" spans="1:28" ht="20" customHeight="1">
+      <c r="A6" s="58"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+    </row>
+    <row r="7" spans="1:28">
+      <c r="A7" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="54"/>
-      <c r="H1" s="62" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-    </row>
-    <row r="2" spans="1:28" ht="20">
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="67"/>
-      <c r="L2" s="66" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="62"/>
-    </row>
-    <row r="3" spans="1:28" ht="21" customHeight="1">
-      <c r="A3" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62">
-        <v>0.02</v>
-      </c>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62">
-        <v>5.85</v>
-      </c>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62">
-        <v>22900</v>
-      </c>
-      <c r="M3" s="62"/>
-    </row>
-    <row r="4" spans="1:28" ht="15" customHeight="1">
-      <c r="A4" s="62"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="62"/>
-      <c r="M4" s="62"/>
-    </row>
-    <row r="5" spans="1:28" ht="20" customHeight="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-    </row>
-    <row r="6" spans="1:28" ht="20" customHeight="1">
-      <c r="A6" s="62"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
-    </row>
-    <row r="7" spans="1:28">
-      <c r="A7" s="56" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="8" spans="1:28" ht="20">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="20">
+      <c r="A9" s="46" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="20">
-      <c r="A9" s="50" t="s">
+    <row r="10" spans="1:28" ht="20">
+      <c r="A10" s="46" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="20">
-      <c r="A10" s="50" t="s">
+    <row r="11" spans="1:28" ht="20">
+      <c r="A11" s="46" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="20">
-      <c r="A11" s="50" t="s">
+    <row r="12" spans="1:28" ht="20">
+      <c r="A12" s="46" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="20">
-      <c r="A12" s="50" t="s">
-        <v>21</v>
-      </c>
-    </row>
     <row r="13" spans="1:28" ht="16" customHeight="1" thickBot="1">
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="65" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="65"/>
-      <c r="M13" s="65"/>
-      <c r="N13" s="65"/>
-      <c r="O13" s="65"/>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="65"/>
-      <c r="R13" s="59"/>
-      <c r="S13" s="59"/>
-      <c r="T13" s="59"/>
-      <c r="U13" s="59"/>
-      <c r="V13" s="59"/>
-      <c r="W13" s="59"/>
-      <c r="X13" s="59"/>
-      <c r="Y13" s="59"/>
-      <c r="Z13" s="59"/>
-      <c r="AA13" s="59"/>
-      <c r="AB13" s="59"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="61"/>
+      <c r="N13" s="61"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="61"/>
+      <c r="Q13" s="61"/>
+      <c r="R13" s="55"/>
+      <c r="S13" s="55"/>
+      <c r="T13" s="55"/>
+      <c r="U13" s="55"/>
+      <c r="V13" s="55"/>
+      <c r="W13" s="55"/>
+      <c r="X13" s="55"/>
+      <c r="Y13" s="55"/>
+      <c r="Z13" s="55"/>
+      <c r="AA13" s="55"/>
+      <c r="AB13" s="55"/>
     </row>
     <row r="14" spans="1:28" ht="31" customHeight="1" thickBot="1">
-      <c r="B14" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="64"/>
+      <c r="B14" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="60"/>
       <c r="D14" s="6" t="s">
         <v>0</v>
       </c>
@@ -1183,104 +1239,104 @@
         <v>1</v>
       </c>
       <c r="J14" s="16"/>
-      <c r="N14" s="23" t="s">
+      <c r="N14" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="24"/>
-      <c r="S14" s="30" t="s">
+      <c r="O14" s="23"/>
+      <c r="S14" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="T14" s="31"/>
-      <c r="X14" s="37" t="s">
+      <c r="T14" s="29"/>
+      <c r="X14" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="Y14" s="38"/>
-      <c r="Z14" s="38"/>
-    </row>
-    <row r="15" spans="1:28" ht="91" thickBot="1">
-      <c r="A15" s="57" t="s">
-        <v>28</v>
+      <c r="Y14" s="35"/>
+      <c r="Z14" s="35"/>
+    </row>
+    <row r="15" spans="1:28" ht="106" thickBot="1">
+      <c r="A15" s="53" t="s">
+        <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="57" t="s">
-        <v>13</v>
+        <v>31</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>12</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="I15" s="18" t="s">
         <v>10</v>
       </c>
       <c r="J15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="L15" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="M15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="N15" s="26" t="s">
+      <c r="N15" s="25" t="s">
         <v>10</v>
       </c>
       <c r="O15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="P15" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q15" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="R15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S15" s="33" t="s">
+      <c r="S15" s="31" t="s">
         <v>10</v>
       </c>
       <c r="T15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="V15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="W15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="U15" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="V15" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="W15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="X15" s="40" t="s">
+      <c r="X15" s="37" t="s">
         <v>10</v>
       </c>
       <c r="Y15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB15" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="Z15" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA15" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB15" s="10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="41" customHeight="1" thickBot="1">
@@ -1315,11 +1371,11 @@
       <c r="I16" s="18">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="J16" s="20">
+      <c r="J16" s="19">
         <f>(I16-AVERAGE($D16,$I16,$N16,$S16,$X16))/STDEV($D16,$I16,$N16,$S16,$X16)</f>
         <v>-1.6298051341843633</v>
       </c>
-      <c r="K16" s="21">
+      <c r="K16" s="20">
         <f>100*L16/$C16</f>
         <v>3.4756637800451569</v>
       </c>
@@ -1330,54 +1386,54 @@
         <f>(K16-AVERAGE($F16,$K16,$P16,$U16,$Z16))/STDEV($F16,$K16,$P16,$U16,$Z16)</f>
         <v>-1.7209293946365365</v>
       </c>
-      <c r="N16" s="26">
+      <c r="N16" s="25">
         <v>1.84E-2</v>
       </c>
-      <c r="O16" s="49">
+      <c r="O16" s="45">
         <f>(N16-AVERAGE($D16,$I16,$N16,$S16,$X16))/STDEV($D16,$I16,$N16,$S16,$X16)</f>
         <v>0.83027808722599616</v>
       </c>
-      <c r="P16" s="29">
+      <c r="P16" s="27">
         <f>100*Q16/$C16</f>
         <v>5.6700677355740376</v>
       </c>
-      <c r="Q16" s="26">
+      <c r="Q16" s="25">
         <v>19839</v>
       </c>
-      <c r="R16" s="47">
+      <c r="R16" s="43">
         <f>(P16-AVERAGE($F16,$K16,$P16,$U16,$Z16))/STDEV($F16,$K16,$P16,$U16,$Z16)</f>
         <v>0.83108232740057075</v>
       </c>
-      <c r="S16" s="33">
+      <c r="S16" s="31">
         <v>1.8100000000000002E-2</v>
       </c>
-      <c r="T16" s="35">
+      <c r="T16" s="32">
         <f>(S16-AVERAGE($D16,$I16,$N16,$S16,$X16))/STDEV($D16,$I16,$N16,$S16,$X16)</f>
         <v>0.6765228858878497</v>
       </c>
-      <c r="U16" s="36">
+      <c r="U16" s="33">
         <f>100*V16/$C16</f>
         <v>5.3645431421303842</v>
       </c>
-      <c r="V16" s="33">
+      <c r="V16" s="31">
         <v>18770</v>
       </c>
       <c r="W16" s="11">
         <f>(U16-AVERAGE($F16,$K16,$P16,$U16,$Z16))/STDEV($F16,$K16,$P16,$U16,$Z16)</f>
         <v>0.47576837443656128</v>
       </c>
-      <c r="X16" s="40">
+      <c r="X16" s="37">
         <v>1.6299999999999999E-2</v>
       </c>
-      <c r="Y16" s="42">
+      <c r="Y16" s="38">
         <f>(X16-AVERAGE($D16,$I16,$N16,$S16,$X16))/STDEV($D16,$I16,$N16,$S16,$X16)</f>
         <v>-0.24600832214103657</v>
       </c>
-      <c r="Z16" s="43">
+      <c r="Z16" s="39">
         <f>100*AA16/$C16</f>
         <v>5.0187201691960333</v>
       </c>
-      <c r="AA16" s="45">
+      <c r="AA16" s="41">
         <v>17560</v>
       </c>
       <c r="AB16" s="11">
@@ -1399,90 +1455,90 @@
       <c r="D17" s="9">
         <v>2.2599999999999999E-2</v>
       </c>
-      <c r="E17" s="47">
+      <c r="E17" s="43">
         <f t="shared" ref="E17:E19" si="1">(D17-AVERAGE($D17,$I17,$N17,$S17,$X17))/STDEV($D17,$I17,$N17,$S17,$X17)</f>
         <v>0.72101171653559248</v>
       </c>
       <c r="F17" s="12">
-        <f t="shared" ref="F17:F18" si="2">100*G17/$C17</f>
+        <f t="shared" ref="F17:F19" si="2">100*G17/$C17</f>
         <v>6.5922756080385678</v>
       </c>
       <c r="G17" s="9">
         <v>26774</v>
       </c>
-      <c r="H17" s="47">
+      <c r="H17" s="43">
         <f t="shared" ref="H17:H19" si="3">(F17-AVERAGE($F17,$K17,$P17,$U17,$Z17))/STDEV($F17,$K17,$P17,$U17,$Z17)</f>
         <v>1.043673703127016</v>
       </c>
       <c r="I17" s="18">
         <v>1.55E-2</v>
       </c>
-      <c r="J17" s="20">
+      <c r="J17" s="19">
         <f t="shared" ref="J17:J19" si="4">(I17-AVERAGE($D17,$I17,$N17,$S17,$X17))/STDEV($D17,$I17,$N17,$S17,$X17)</f>
         <v>-1.7640286656987272</v>
       </c>
-      <c r="K17" s="21">
+      <c r="K17" s="20">
         <f>100*L17/$C17</f>
         <v>3.5962791338989812</v>
       </c>
-      <c r="L17" s="22">
+      <c r="L17" s="21">
         <v>14606</v>
       </c>
       <c r="M17" s="11">
         <f t="shared" ref="M17:M19" si="5">(K17-AVERAGE($F17,$K17,$P17,$U17,$Z17))/STDEV($F17,$K17,$P17,$U17,$Z17)</f>
         <v>-1.6670976466957144</v>
       </c>
-      <c r="N17" s="26">
+      <c r="N17" s="25">
         <v>2.1399999999999999E-2</v>
       </c>
-      <c r="O17" s="28">
+      <c r="O17" s="26">
         <f t="shared" ref="O17:O19" si="6">(N17-AVERAGE($D17,$I17,$N17,$S17,$X17))/STDEV($D17,$I17,$N17,$S17,$X17)</f>
         <v>0.30100489136922859</v>
       </c>
-      <c r="P17" s="29">
+      <c r="P17" s="27">
         <f t="shared" ref="P17:P18" si="7">100*Q17/$C17</f>
         <v>5.6283270383264963</v>
       </c>
-      <c r="Q17" s="26">
+      <c r="Q17" s="25">
         <v>22859</v>
       </c>
       <c r="R17" s="11">
         <f t="shared" ref="R17:R19" si="8">(P17-AVERAGE($F17,$K17,$P17,$U17,$Z17))/STDEV($F17,$K17,$P17,$U17,$Z17)</f>
         <v>0.17149505137192111</v>
       </c>
-      <c r="S17" s="33">
+      <c r="S17" s="31">
         <v>2.1700000000000001E-2</v>
       </c>
-      <c r="T17" s="35">
+      <c r="T17" s="32">
         <f t="shared" ref="T17:T19" si="9">(S17-AVERAGE($D17,$I17,$N17,$S17,$X17))/STDEV($D17,$I17,$N17,$S17,$X17)</f>
         <v>0.4060065976608202</v>
       </c>
-      <c r="U17" s="36">
+      <c r="U17" s="33">
         <f t="shared" ref="U17:U19" si="10">100*V17/$C17</f>
         <v>5.6888969867681745</v>
       </c>
-      <c r="V17" s="33">
+      <c r="V17" s="31">
         <v>23105</v>
       </c>
-      <c r="W17" s="48">
+      <c r="W17" s="44">
         <f t="shared" ref="W17:W19" si="11">(U17-AVERAGE($F17,$K17,$P17,$U17,$Z17))/STDEV($F17,$K17,$P17,$U17,$Z17)</f>
         <v>0.22629861416419536</v>
       </c>
-      <c r="X17" s="40">
+      <c r="X17" s="37">
         <v>2.1499999999999998E-2</v>
       </c>
-      <c r="Y17" s="42">
+      <c r="Y17" s="38">
         <f>(X17-AVERAGE($D17,$I17,$N17,$S17,$X17))/STDEV($D17,$I17,$N17,$S17,$X17)</f>
         <v>0.33600546013309207</v>
       </c>
-      <c r="Z17" s="43">
+      <c r="Z17" s="39">
         <f t="shared" ref="Z17:Z18" si="12">100*AA17/$C17</f>
         <v>5.6881583288603492</v>
       </c>
-      <c r="AA17" s="45">
+      <c r="AA17" s="41">
         <v>23102</v>
       </c>
-      <c r="AB17" s="48">
+      <c r="AB17" s="44">
         <f>(Z17-AVERAGE($F17,$K17,$P17,$U17,$Z17))/STDEV($F17,$K17,$P17,$U17,$Z17)</f>
         <v>0.22563027803258237</v>
       </c>
@@ -1519,11 +1575,11 @@
       <c r="I18" s="15">
         <v>2.1100000000000001E-2</v>
       </c>
-      <c r="J18" s="20">
+      <c r="J18" s="19">
         <f t="shared" si="4"/>
         <v>-0.52666037785524866</v>
       </c>
-      <c r="K18" s="21">
+      <c r="K18" s="20">
         <f>100*L18/$C18</f>
         <v>5.8862771778696095</v>
       </c>
@@ -1534,54 +1590,54 @@
         <f t="shared" si="5"/>
         <v>-0.580561186437208</v>
       </c>
-      <c r="N18" s="23">
+      <c r="N18" s="22">
         <v>2.46E-2</v>
       </c>
-      <c r="O18" s="49">
+      <c r="O18" s="45">
         <f t="shared" si="6"/>
         <v>0.71882024545108369</v>
       </c>
-      <c r="P18" s="29">
+      <c r="P18" s="27">
         <f t="shared" si="7"/>
         <v>7.3192620379464346</v>
       </c>
-      <c r="Q18" s="23">
+      <c r="Q18" s="22">
         <v>27648</v>
       </c>
-      <c r="R18" s="47">
+      <c r="R18" s="43">
         <f t="shared" si="8"/>
         <v>0.75852936332613441</v>
       </c>
-      <c r="S18" s="30">
+      <c r="S18" s="28">
         <v>2.4400000000000002E-2</v>
       </c>
-      <c r="T18" s="35">
+      <c r="T18" s="32">
         <f t="shared" si="9"/>
         <v>0.64764992411929367</v>
       </c>
-      <c r="U18" s="36">
+      <c r="U18" s="33">
         <f t="shared" si="10"/>
         <v>7.1212438086212053</v>
       </c>
-      <c r="V18" s="30">
+      <c r="V18" s="28">
         <v>26900</v>
       </c>
       <c r="W18" s="11">
         <f t="shared" si="11"/>
         <v>0.57348599897679375</v>
       </c>
-      <c r="X18" s="37">
+      <c r="X18" s="34">
         <v>2.4500000000000001E-2</v>
       </c>
-      <c r="Y18" s="42">
+      <c r="Y18" s="38">
         <f>(X18-AVERAGE($D18,$I18,$N18,$S18,$X18))/STDEV($D18,$I18,$N18,$S18,$X18)</f>
         <v>0.68323508478518868</v>
       </c>
-      <c r="Z18" s="43">
+      <c r="Z18" s="39">
         <f t="shared" si="12"/>
         <v>7.2962305059259869</v>
       </c>
-      <c r="AA18" s="46">
+      <c r="AA18" s="42">
         <v>27561</v>
       </c>
       <c r="AB18" s="11">
@@ -1595,7 +1651,7 @@
       </c>
       <c r="B19" s="4">
         <f t="shared" si="0"/>
-        <v>2.9879526963784286</v>
+        <v>3.3420332637338901</v>
       </c>
       <c r="C19" s="1">
         <v>444448</v>
@@ -1608,24 +1664,24 @@
         <v>-0.66066711216103557</v>
       </c>
       <c r="F19" s="12">
-        <f t="shared" ref="F19" si="13">G19/$C19</f>
-        <v>1.7882856937144503E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.7882856937144502</v>
       </c>
       <c r="G19" s="6">
         <v>7948</v>
       </c>
       <c r="H19" s="11">
         <f t="shared" si="3"/>
-        <v>-1.2550273072092135</v>
+        <v>-0.81909513840465953</v>
       </c>
       <c r="I19" s="15">
         <v>6.1999999999999998E-3</v>
       </c>
-      <c r="J19" s="20">
+      <c r="J19" s="19">
         <f t="shared" si="4"/>
         <v>-1.4441505464545716</v>
       </c>
-      <c r="K19" s="21">
+      <c r="K19" s="20">
         <f>100*L19/$C19</f>
         <v>0.81179350565195474</v>
       </c>
@@ -1634,70 +1690,70 @@
       </c>
       <c r="M19" s="11">
         <f t="shared" si="5"/>
-        <v>-0.91955386803624695</v>
-      </c>
-      <c r="N19" s="23">
+        <v>-1.3338763160975786</v>
+      </c>
+      <c r="N19" s="22">
         <v>1.6400000000000001E-2</v>
       </c>
-      <c r="O19" s="49">
+      <c r="O19" s="45">
         <f t="shared" si="6"/>
         <v>0.71572270484112221</v>
       </c>
-      <c r="P19" s="29">
+      <c r="P19" s="27">
         <f>100*Q19/$C19</f>
         <v>4.7816617467060265</v>
       </c>
-      <c r="Q19" s="23">
+      <c r="Q19" s="22">
         <v>21252</v>
       </c>
-      <c r="R19" s="47">
+      <c r="R19" s="43">
         <f t="shared" si="8"/>
-        <v>0.75794643259059435</v>
-      </c>
-      <c r="S19" s="30">
+        <v>0.75893453625584661</v>
+      </c>
+      <c r="S19" s="28">
         <v>1.6199999999999999E-2</v>
       </c>
-      <c r="T19" s="35">
+      <c r="T19" s="32">
         <f t="shared" si="9"/>
         <v>0.673372248933363</v>
       </c>
-      <c r="U19" s="36">
+      <c r="U19" s="33">
         <f t="shared" si="10"/>
         <v>4.6012131902944775</v>
       </c>
-      <c r="V19" s="30">
+      <c r="V19" s="28">
         <v>20450</v>
       </c>
       <c r="W19" s="11">
         <f t="shared" si="11"/>
-        <v>0.68169641892573785</v>
-      </c>
-      <c r="X19" s="37">
+        <v>0.66380677023978163</v>
+      </c>
+      <c r="X19" s="34">
         <v>1.6400000000000001E-2</v>
       </c>
-      <c r="Y19" s="51">
+      <c r="Y19" s="47">
         <f>(X19-AVERAGE($D19,$I19,$N19,$S19,$X19))/STDEV($D19,$I19,$N19,$S19,$X19)</f>
         <v>0.71572270484112221</v>
       </c>
-      <c r="Z19" s="43">
+      <c r="Z19" s="39">
         <f>100*AA19/$C19</f>
         <v>4.7272121823025417</v>
       </c>
-      <c r="AA19" s="44">
+      <c r="AA19" s="40">
         <v>21010</v>
       </c>
       <c r="AB19" s="11">
         <f>(Z19-AVERAGE($F19,$K19,$P19,$U19,$Z19))/STDEV($F19,$K19,$P19,$U19,$Z19)</f>
-        <v>0.73493832372912893</v>
+        <v>0.73023014800661001</v>
       </c>
     </row>
     <row r="20" spans="1:28" ht="21" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="60">
+      <c r="B20" s="56">
         <f>AVERAGE(B16:B19)</f>
-        <v>4.9724323476735366</v>
+        <v>5.0609524895124016</v>
       </c>
       <c r="C20" s="5">
         <f>AVERAGE(C16:C19)</f>
@@ -1708,100 +1764,100 @@
         <v>1.7075E-2</v>
       </c>
       <c r="E20" s="13">
-        <f t="shared" ref="E20:AB20" si="14">AVERAGE(E16:E19)</f>
+        <f t="shared" ref="E20:AB20" si="13">AVERAGE(E16:E19)</f>
         <v>-0.27342194722855073</v>
       </c>
       <c r="F20" s="13">
-        <f t="shared" si="14"/>
-        <v>4.1932741208382209</v>
+        <f t="shared" si="13"/>
+        <v>4.635874830032547</v>
       </c>
       <c r="G20" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>17912.5</v>
       </c>
       <c r="H20" s="13">
-        <f t="shared" si="14"/>
-        <v>-0.33983122594384818</v>
+        <f t="shared" si="13"/>
+        <v>-0.23084818374270968</v>
       </c>
       <c r="I20" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1.41E-2</v>
       </c>
       <c r="J20" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>-1.3411611810482276</v>
       </c>
       <c r="K20" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>3.4425033993664256</v>
       </c>
       <c r="L20" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>13152.5</v>
       </c>
       <c r="M20" s="13">
-        <f t="shared" si="14"/>
-        <v>-1.2220355239514265</v>
-      </c>
-      <c r="N20" s="52">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
+        <v>-1.3256161359667593</v>
+      </c>
+      <c r="N20" s="48">
+        <f t="shared" si="13"/>
         <v>2.0199999999999999E-2</v>
       </c>
-      <c r="O20" s="53">
-        <f t="shared" si="14"/>
+      <c r="O20" s="49">
+        <f t="shared" si="13"/>
         <v>0.64145648222185769</v>
       </c>
-      <c r="P20" s="52">
-        <f t="shared" si="14"/>
+      <c r="P20" s="48">
+        <f t="shared" si="13"/>
         <v>5.8498296396382479</v>
       </c>
       <c r="Q20" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>22899.5</v>
       </c>
-      <c r="R20" s="53">
+      <c r="R20" s="49">
         <f>AVERAGE(R16:R19)</f>
-        <v>0.62976329367230521</v>
+        <v>0.6300103195886182</v>
       </c>
       <c r="S20" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>2.01E-2</v>
       </c>
       <c r="T20" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0.6008879141503316</v>
       </c>
       <c r="U20" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>5.6939742819535599</v>
       </c>
       <c r="V20" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>22306.25</v>
       </c>
       <c r="W20" s="13">
-        <f t="shared" si="14"/>
-        <v>0.4893123516258221</v>
+        <f t="shared" si="13"/>
+        <v>0.48483993945433301</v>
       </c>
       <c r="X20" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1.9675000000000002E-2</v>
       </c>
       <c r="Y20" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0.37223873190459156</v>
       </c>
       <c r="Z20" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>5.6825802965712278</v>
       </c>
       <c r="AA20" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>22308.25</v>
       </c>
       <c r="AB20" s="13">
-        <f t="shared" si="14"/>
-        <v>0.4427911045971491</v>
+        <f t="shared" si="13"/>
+        <v>0.44161406066651937</v>
       </c>
     </row>
   </sheetData>
@@ -1831,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U15" sqref="U15:V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1841,188 +1897,188 @@
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="8" customWidth="1"/>
+    <col min="5" max="5" width="11" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" style="8" customWidth="1"/>
     <col min="8" max="8" width="9" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="17" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="17" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.1640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" style="25" customWidth="1"/>
-    <col min="18" max="18" width="9.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.83203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9" style="32" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="32" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="32" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.33203125" style="39" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.83203125" style="39" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9" style="39" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.1640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9" style="39" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="24" customWidth="1"/>
+    <col min="18" max="18" width="9.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.83203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" style="30" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.1640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" style="30" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.83203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" style="36" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9" style="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="20" customHeight="1">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="54"/>
-      <c r="H1" s="62" t="s">
+      <c r="A1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="50"/>
+      <c r="H1" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+    </row>
+    <row r="2" spans="1:28" ht="20">
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-    </row>
-    <row r="2" spans="1:28" ht="20">
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="62" t="s">
+      <c r="I2" s="58"/>
+      <c r="J2" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="67"/>
-      <c r="L2" s="66" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="62"/>
+      <c r="M2" s="58"/>
     </row>
     <row r="3" spans="1:28" ht="21" customHeight="1">
-      <c r="A3" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
+      <c r="A3" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
     </row>
     <row r="4" spans="1:28" ht="15" customHeight="1">
-      <c r="A4" s="62"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="62"/>
-      <c r="M4" s="62"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
     </row>
     <row r="5" spans="1:28" ht="20" customHeight="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
     </row>
     <row r="6" spans="1:28" ht="20" customHeight="1">
-      <c r="A6" s="62"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
     </row>
     <row r="7" spans="1:28">
-      <c r="A7" s="56" t="s">
-        <v>27</v>
+      <c r="A7" s="52" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="20">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="46" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="20">
+      <c r="A9" s="46" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="20">
-      <c r="A9" s="50" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="10" spans="1:28" ht="20">
-      <c r="A10" s="50"/>
+      <c r="A10" s="46"/>
     </row>
     <row r="11" spans="1:28" ht="20">
-      <c r="A11" s="50"/>
+      <c r="A11" s="46"/>
     </row>
     <row r="12" spans="1:28" ht="20">
-      <c r="A12" s="50"/>
+      <c r="A12" s="46"/>
     </row>
     <row r="13" spans="1:28" ht="16" customHeight="1" thickBot="1">
-      <c r="C13" s="58" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="65"/>
-      <c r="M13" s="65"/>
-      <c r="N13" s="65"/>
-      <c r="O13" s="65"/>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="65"/>
-      <c r="R13" s="59"/>
-      <c r="S13" s="59"/>
-      <c r="T13" s="59"/>
-      <c r="U13" s="59"/>
-      <c r="V13" s="59"/>
-      <c r="W13" s="59"/>
-      <c r="X13" s="59"/>
-      <c r="Y13" s="59"/>
-      <c r="Z13" s="59"/>
-      <c r="AA13" s="59"/>
-      <c r="AB13" s="59"/>
+      <c r="C13" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="61"/>
+      <c r="N13" s="61"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="61"/>
+      <c r="Q13" s="61"/>
+      <c r="R13" s="55"/>
+      <c r="S13" s="55"/>
+      <c r="T13" s="55"/>
+      <c r="U13" s="55"/>
+      <c r="V13" s="55"/>
+      <c r="W13" s="55"/>
+      <c r="X13" s="55"/>
+      <c r="Y13" s="55"/>
+      <c r="Z13" s="55"/>
+      <c r="AA13" s="55"/>
+      <c r="AB13" s="55"/>
     </row>
     <row r="14" spans="1:28" ht="31" customHeight="1" thickBot="1">
-      <c r="B14" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="64"/>
+      <c r="B14" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="60"/>
       <c r="D14" s="6" t="s">
         <v>0</v>
       </c>
@@ -2031,104 +2087,104 @@
         <v>1</v>
       </c>
       <c r="J14" s="16"/>
-      <c r="N14" s="23" t="s">
+      <c r="N14" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="24"/>
-      <c r="S14" s="30" t="s">
+      <c r="O14" s="23"/>
+      <c r="S14" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="T14" s="31"/>
-      <c r="X14" s="37" t="s">
+      <c r="T14" s="29"/>
+      <c r="X14" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="Y14" s="38"/>
-      <c r="Z14" s="38"/>
-    </row>
-    <row r="15" spans="1:28" ht="91" thickBot="1">
-      <c r="A15" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="57" t="s">
-        <v>13</v>
+      <c r="Y14" s="35"/>
+      <c r="Z14" s="35"/>
+    </row>
+    <row r="15" spans="1:28" ht="106" thickBot="1">
+      <c r="A15" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>12</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="I15" s="18" t="s">
         <v>10</v>
       </c>
       <c r="J15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="L15" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="M15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="N15" s="26" t="s">
+      <c r="N15" s="25" t="s">
         <v>10</v>
       </c>
       <c r="O15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="P15" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q15" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="R15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="S15" s="33" t="s">
+      <c r="S15" s="31" t="s">
         <v>10</v>
       </c>
       <c r="T15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="V15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="W15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="U15" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="V15" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="W15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="X15" s="40" t="s">
+      <c r="X15" s="37" t="s">
         <v>10</v>
       </c>
       <c r="Y15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB15" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="Z15" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA15" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB15" s="10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="41" customHeight="1" thickBot="1">
@@ -2137,84 +2193,88 @@
       </c>
       <c r="B16" s="4">
         <f>AVERAGE(F16,K16,P16,U16,Z16)</f>
-        <v>1.0496441738832205</v>
+        <v>2.2519649032553088</v>
       </c>
       <c r="C16" s="2">
         <v>349890</v>
       </c>
-      <c r="D16" s="9">
-        <v>1.7500000000000002E-2</v>
-      </c>
-      <c r="E16" s="11" t="e">
-        <f>(D16-AVERAGE($D16,$I16,$N16,$S16,$X16))/STDEV($D16,$I16,$N16,$S16,$X16)</f>
-        <v>#DIV/0!</v>
+      <c r="D16" s="25">
+        <v>1.84E-2</v>
+      </c>
+      <c r="E16" s="11">
+        <f>(D16-AVERAGE($D16,$I16))/STDEV($D16,$I16)</f>
+        <v>0.70710678118654757</v>
       </c>
       <c r="F16" s="12">
         <f>100*G16/$C16</f>
-        <v>5.2482208694161026</v>
-      </c>
-      <c r="G16" s="9">
-        <v>18363</v>
+        <v>5.6700677355740376</v>
+      </c>
+      <c r="G16" s="25">
+        <v>19839</v>
       </c>
       <c r="H16" s="11">
         <f>(F16-AVERAGE($F16,$K16,$P16,$U16,$Z16))/STDEV($F16,$K16,$P16,$U16,$Z16)</f>
-        <v>1.7888543819998317</v>
-      </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="20" t="e">
+        <v>1.1084202709591282</v>
+      </c>
+      <c r="I16" s="18">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="J16" s="19">
         <f>(I16-AVERAGE($D16,$I16,$N16,$S16,$X16))/STDEV($D16,$I16,$N16,$S16,$X16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K16" s="21">
+        <v>-0.70710678118654757</v>
+      </c>
+      <c r="K16" s="20">
         <f>100*L16/$C16</f>
-        <v>0</v>
-      </c>
-      <c r="L16" s="18"/>
+        <v>5.5897567807025066</v>
+      </c>
+      <c r="L16" s="18">
+        <v>19558</v>
+      </c>
       <c r="M16" s="11">
         <f>(K16-AVERAGE($F16,$K16,$P16,$U16,$Z16))/STDEV($F16,$K16,$P16,$U16,$Z16)</f>
-        <v>-0.44721359549995793</v>
-      </c>
-      <c r="N16" s="26"/>
-      <c r="O16" s="49" t="e">
+        <v>1.0823770842188094</v>
+      </c>
+      <c r="N16" s="25"/>
+      <c r="O16" s="45">
         <f>(N16-AVERAGE($D16,$I16,$N16,$S16,$X16))/STDEV($D16,$I16,$N16,$S16,$X16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P16" s="29">
+        <v>-129.40054095713899</v>
+      </c>
+      <c r="P16" s="27">
         <f>100*Q16/$C16</f>
         <v>0</v>
       </c>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="47">
+      <c r="Q16" s="25"/>
+      <c r="R16" s="43">
         <f>(P16-AVERAGE($F16,$K16,$P16,$U16,$Z16))/STDEV($F16,$K16,$P16,$U16,$Z16)</f>
-        <v>-0.44721359549995793</v>
-      </c>
-      <c r="S16" s="33"/>
-      <c r="T16" s="35" t="e">
+        <v>-0.7302657850593125</v>
+      </c>
+      <c r="S16" s="31"/>
+      <c r="T16" s="32">
         <f>(S16-AVERAGE($D16,$I16,$N16,$S16,$X16))/STDEV($D16,$I16,$N16,$S16,$X16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U16" s="36">
+        <v>-129.40054095713899</v>
+      </c>
+      <c r="U16" s="33">
         <f>100*V16/$C16</f>
         <v>0</v>
       </c>
-      <c r="V16" s="33"/>
+      <c r="V16" s="31"/>
       <c r="W16" s="11">
         <f>(U16-AVERAGE($F16,$K16,$P16,$U16,$Z16))/STDEV($F16,$K16,$P16,$U16,$Z16)</f>
-        <v>-0.44721359549995793</v>
-      </c>
-      <c r="X16" s="40"/>
-      <c r="Y16" s="42" t="e">
+        <v>-0.7302657850593125</v>
+      </c>
+      <c r="X16" s="37"/>
+      <c r="Y16" s="38">
         <f>(X16-AVERAGE($D16,$I16,$N16,$S16,$X16))/STDEV($D16,$I16,$N16,$S16,$X16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z16" s="43">
+        <v>-129.40054095713899</v>
+      </c>
+      <c r="Z16" s="39">
         <f>100*AA16/$C16</f>
         <v>0</v>
       </c>
-      <c r="AA16" s="45"/>
+      <c r="AA16" s="41"/>
       <c r="AB16" s="11">
         <f>(Z16-AVERAGE($F16,$K16,$P16,$U16,$Z16))/STDEV($F16,$K16,$P16,$U16,$Z16)</f>
-        <v>-0.44721359549995793</v>
+        <v>-0.7302657850593125</v>
       </c>
     </row>
     <row r="17" spans="1:28" ht="61" thickBot="1">
@@ -2223,84 +2283,88 @@
       </c>
       <c r="B17" s="4">
         <f t="shared" ref="B17:B19" si="0">AVERAGE(F17,K17,P17,U17,Z17)</f>
-        <v>1.3184551216077136</v>
+        <v>2.2657100226029323</v>
       </c>
       <c r="C17" s="2">
         <v>406142</v>
       </c>
-      <c r="D17" s="9">
-        <v>2.2599999999999999E-2</v>
-      </c>
-      <c r="E17" s="47" t="e">
-        <f t="shared" ref="E17:E19" si="1">(D17-AVERAGE($D17,$I17,$N17,$S17,$X17))/STDEV($D17,$I17,$N17,$S17,$X17)</f>
+      <c r="D17" s="18">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="E17" s="44" t="e">
+        <f>(D17-AVERAGE($D17,$I17,$N17,$S17,$X17))/STDEV($D17,$I17,$N17,$S17,$X17)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F17" s="12">
-        <f t="shared" ref="F17:F18" si="2">100*G17/$C17</f>
-        <v>6.5922756080385678</v>
-      </c>
-      <c r="G17" s="9">
-        <v>26774</v>
-      </c>
-      <c r="H17" s="47">
-        <f t="shared" ref="H17:H19" si="3">(F17-AVERAGE($F17,$K17,$P17,$U17,$Z17))/STDEV($F17,$K17,$P17,$U17,$Z17)</f>
-        <v>1.7888543819998317</v>
-      </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="20" t="e">
-        <f t="shared" ref="J17:J19" si="4">(I17-AVERAGE($D17,$I17,$N17,$S17,$X17))/STDEV($D17,$I17,$N17,$S17,$X17)</f>
+        <f t="shared" ref="F17:F19" si="1">100*G17/$C17</f>
+        <v>5.6642750565073303</v>
+      </c>
+      <c r="G17" s="65">
+        <v>23005</v>
+      </c>
+      <c r="H17" s="44">
+        <f t="shared" ref="H17:H19" si="2">(F17-AVERAGE($F17,$K17,$P17,$U17,$Z17))/STDEV($F17,$K17,$P17,$U17,$Z17)</f>
+        <v>1.0954451150103321</v>
+      </c>
+      <c r="I17" s="18">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="J17" s="19" t="e">
+        <f>(I17-AVERAGE($D17,$I17,$N17,$S17,$X17))/STDEV($D17,$I17,$N17,$S17,$X17)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K17" s="21">
+      <c r="K17" s="20">
         <f>100*L17/$C17</f>
+        <v>5.6642750565073303</v>
+      </c>
+      <c r="L17" s="65">
+        <v>23005</v>
+      </c>
+      <c r="M17" s="11">
+        <f t="shared" ref="M17:M19" si="3">(K17-AVERAGE($F17,$K17,$P17,$U17,$Z17))/STDEV($F17,$K17,$P17,$U17,$Z17)</f>
+        <v>1.0954451150103321</v>
+      </c>
+      <c r="N17" s="25"/>
+      <c r="O17" s="26" t="e">
+        <f t="shared" ref="O17:O19" si="4">(N17-AVERAGE($D17,$I17,$N17,$S17,$X17))/STDEV($D17,$I17,$N17,$S17,$X17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P17" s="27">
+        <f t="shared" ref="P17:P18" si="5">100*Q17/$C17</f>
         <v>0</v>
       </c>
-      <c r="L17" s="22"/>
-      <c r="M17" s="11">
-        <f t="shared" ref="M17:M19" si="5">(K17-AVERAGE($F17,$K17,$P17,$U17,$Z17))/STDEV($F17,$K17,$P17,$U17,$Z17)</f>
-        <v>-0.44721359549995793</v>
-      </c>
-      <c r="N17" s="26"/>
-      <c r="O17" s="28" t="e">
-        <f t="shared" ref="O17:O19" si="6">(N17-AVERAGE($D17,$I17,$N17,$S17,$X17))/STDEV($D17,$I17,$N17,$S17,$X17)</f>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="11">
+        <f t="shared" ref="R17:R19" si="6">(P17-AVERAGE($F17,$K17,$P17,$U17,$Z17))/STDEV($F17,$K17,$P17,$U17,$Z17)</f>
+        <v>-0.73029674334022154</v>
+      </c>
+      <c r="S17" s="31"/>
+      <c r="T17" s="32" t="e">
+        <f t="shared" ref="T17:T19" si="7">(S17-AVERAGE($D17,$I17,$N17,$S17,$X17))/STDEV($D17,$I17,$N17,$S17,$X17)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P17" s="29">
-        <f t="shared" ref="P17:P18" si="7">100*Q17/$C17</f>
+      <c r="U17" s="33">
+        <f t="shared" ref="U17:U19" si="8">100*V17/$C17</f>
         <v>0</v>
       </c>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="11">
-        <f t="shared" ref="R17:R19" si="8">(P17-AVERAGE($F17,$K17,$P17,$U17,$Z17))/STDEV($F17,$K17,$P17,$U17,$Z17)</f>
-        <v>-0.44721359549995793</v>
-      </c>
-      <c r="S17" s="33"/>
-      <c r="T17" s="35" t="e">
-        <f t="shared" ref="T17:T19" si="9">(S17-AVERAGE($D17,$I17,$N17,$S17,$X17))/STDEV($D17,$I17,$N17,$S17,$X17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U17" s="36">
-        <f t="shared" ref="U17:U19" si="10">100*V17/$C17</f>
-        <v>0</v>
-      </c>
-      <c r="V17" s="33"/>
-      <c r="W17" s="48">
-        <f t="shared" ref="W17:W19" si="11">(U17-AVERAGE($F17,$K17,$P17,$U17,$Z17))/STDEV($F17,$K17,$P17,$U17,$Z17)</f>
-        <v>-0.44721359549995793</v>
-      </c>
-      <c r="X17" s="40"/>
-      <c r="Y17" s="42" t="e">
+      <c r="V17" s="31"/>
+      <c r="W17" s="44">
+        <f t="shared" ref="W17:W19" si="9">(U17-AVERAGE($F17,$K17,$P17,$U17,$Z17))/STDEV($F17,$K17,$P17,$U17,$Z17)</f>
+        <v>-0.73029674334022154</v>
+      </c>
+      <c r="X17" s="37"/>
+      <c r="Y17" s="38" t="e">
         <f>(X17-AVERAGE($D17,$I17,$N17,$S17,$X17))/STDEV($D17,$I17,$N17,$S17,$X17)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z17" s="43">
-        <f t="shared" ref="Z17:Z18" si="12">100*AA17/$C17</f>
+      <c r="Z17" s="39">
+        <f t="shared" ref="Z17:Z18" si="10">100*AA17/$C17</f>
         <v>0</v>
       </c>
-      <c r="AA17" s="45"/>
-      <c r="AB17" s="48">
+      <c r="AA17" s="41"/>
+      <c r="AB17" s="44">
         <f>(Z17-AVERAGE($F17,$K17,$P17,$U17,$Z17))/STDEV($F17,$K17,$P17,$U17,$Z17)</f>
-        <v>-0.44721359549995793</v>
+        <v>-0.73029674334022154</v>
       </c>
     </row>
     <row r="18" spans="1:28" ht="41" customHeight="1" thickBot="1">
@@ -2309,84 +2373,88 @@
       </c>
       <c r="B18" s="4">
         <f t="shared" si="0"/>
-        <v>0.98294342979221327</v>
+        <v>2.9428473856563855</v>
       </c>
       <c r="C18" s="1">
         <v>377743</v>
       </c>
-      <c r="D18" s="6">
-        <v>1.83E-2</v>
-      </c>
-      <c r="E18" s="11" t="e">
+      <c r="D18" s="22">
+        <v>2.46E-2</v>
+      </c>
+      <c r="E18" s="11">
+        <f t="shared" ref="E17:E19" si="11">(D18-AVERAGE($D18,$I18,$N18,$S18,$X18))/STDEV($D18,$I18,$N18,$S18,$X18)</f>
+        <v>-0.70710678118654757</v>
+      </c>
+      <c r="F18" s="12">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F18" s="12">
+        <v>7.3192620379464346</v>
+      </c>
+      <c r="G18" s="22">
+        <v>27648</v>
+      </c>
+      <c r="H18" s="11">
         <f t="shared" si="2"/>
-        <v>4.9147171489610662</v>
-      </c>
-      <c r="G18" s="6">
-        <v>18565</v>
-      </c>
-      <c r="H18" s="11">
+        <v>1.0860267059491449</v>
+      </c>
+      <c r="I18" s="15">
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="J18" s="19">
+        <f t="shared" ref="J17:J19" si="12">(I18-AVERAGE($D18,$I18,$N18,$S18,$X18))/STDEV($D18,$I18,$N18,$S18,$X18)</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="K18" s="20">
+        <f>100*L18/$C18</f>
+        <v>7.3949748903354928</v>
+      </c>
+      <c r="L18" s="15">
+        <v>27934</v>
+      </c>
+      <c r="M18" s="11">
         <f t="shared" si="3"/>
-        <v>1.7888543819998317</v>
-      </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="20" t="e">
+        <v>1.1048151860661</v>
+      </c>
+      <c r="N18" s="22"/>
+      <c r="O18" s="45">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K18" s="21">
-        <f>100*L18/$C18</f>
+        <v>-174.65537495307831</v>
+      </c>
+      <c r="P18" s="27">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L18" s="15"/>
-      <c r="M18" s="11">
-        <f t="shared" si="5"/>
-        <v>-0.44721359549995793</v>
-      </c>
-      <c r="N18" s="23"/>
-      <c r="O18" s="49" t="e">
+      <c r="Q18" s="22"/>
+      <c r="R18" s="43">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P18" s="29">
+        <v>-0.73028063067174831</v>
+      </c>
+      <c r="S18" s="28"/>
+      <c r="T18" s="32">
         <f t="shared" si="7"/>
+        <v>-174.65537495307831</v>
+      </c>
+      <c r="U18" s="33">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="47">
-        <f t="shared" si="8"/>
-        <v>-0.44721359549995793</v>
-      </c>
-      <c r="S18" s="30"/>
-      <c r="T18" s="35" t="e">
+      <c r="V18" s="28"/>
+      <c r="W18" s="11">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U18" s="36">
+        <v>-0.73028063067174831</v>
+      </c>
+      <c r="X18" s="34"/>
+      <c r="Y18" s="38">
+        <f>(X18-AVERAGE($D18,$I18,$N18,$S18,$X18))/STDEV($D18,$I18,$N18,$S18,$X18)</f>
+        <v>-174.65537495307831</v>
+      </c>
+      <c r="Z18" s="39">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="V18" s="30"/>
-      <c r="W18" s="11">
-        <f t="shared" si="11"/>
-        <v>-0.44721359549995793</v>
-      </c>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="42" t="e">
-        <f>(X18-AVERAGE($D18,$I18,$N18,$S18,$X18))/STDEV($D18,$I18,$N18,$S18,$X18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z18" s="43">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AA18" s="46"/>
+      <c r="AA18" s="42"/>
       <c r="AB18" s="11">
         <f>(Z18-AVERAGE($F18,$K18,$P18,$U18,$Z18))/STDEV($F18,$K18,$P18,$U18,$Z18)</f>
-        <v>-0.44721359549995793</v>
+        <v>-0.73028063067174831</v>
       </c>
     </row>
     <row r="19" spans="1:28" ht="41" customHeight="1" thickBot="1">
@@ -2395,197 +2463,201 @@
       </c>
       <c r="B19" s="4">
         <f t="shared" si="0"/>
-        <v>3.5765713874289008E-3</v>
+        <v>1.9126646986824105</v>
       </c>
       <c r="C19" s="1">
         <v>444448</v>
       </c>
-      <c r="D19" s="6">
-        <v>9.9000000000000008E-3</v>
+      <c r="D19" s="22">
+        <v>1.6400000000000001E-2</v>
       </c>
       <c r="E19" s="11" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F19" s="12">
         <f t="shared" si="1"/>
+        <v>4.7816617467060265</v>
+      </c>
+      <c r="G19" s="22">
+        <v>21252</v>
+      </c>
+      <c r="H19" s="11">
+        <f t="shared" si="2"/>
+        <v>1.0954451150103324</v>
+      </c>
+      <c r="I19" s="15">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="J19" s="19" t="e">
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F19" s="12">
-        <f t="shared" ref="F19" si="13">G19/$C19</f>
-        <v>1.7882856937144503E-2</v>
-      </c>
-      <c r="G19" s="6">
-        <v>7948</v>
-      </c>
-      <c r="H19" s="11">
+      <c r="K19" s="20">
+        <f>100*L19/$C19</f>
+        <v>4.7816617467060265</v>
+      </c>
+      <c r="L19" s="15">
+        <v>21252</v>
+      </c>
+      <c r="M19" s="11">
         <f t="shared" si="3"/>
-        <v>1.7888543819998319</v>
-      </c>
-      <c r="I19" s="15"/>
-      <c r="J19" s="20" t="e">
+        <v>1.0954451150103324</v>
+      </c>
+      <c r="N19" s="22"/>
+      <c r="O19" s="45" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K19" s="21">
-        <f>100*L19/$C19</f>
-        <v>0</v>
-      </c>
-      <c r="L19" s="15"/>
-      <c r="M19" s="11">
-        <f t="shared" si="5"/>
-        <v>-0.44721359549995798</v>
-      </c>
-      <c r="N19" s="23"/>
-      <c r="O19" s="49" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P19" s="29">
+      <c r="P19" s="27">
         <f>100*Q19/$C19</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="47">
+      <c r="Q19" s="22"/>
+      <c r="R19" s="43">
+        <f t="shared" si="6"/>
+        <v>-0.73029674334022143</v>
+      </c>
+      <c r="S19" s="28"/>
+      <c r="T19" s="32" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U19" s="33">
         <f t="shared" si="8"/>
-        <v>-0.44721359549995798</v>
-      </c>
-      <c r="S19" s="30"/>
-      <c r="T19" s="35" t="e">
+        <v>0</v>
+      </c>
+      <c r="V19" s="28"/>
+      <c r="W19" s="11">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U19" s="36">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="V19" s="30"/>
-      <c r="W19" s="11">
-        <f t="shared" si="11"/>
-        <v>-0.44721359549995798</v>
-      </c>
-      <c r="X19" s="37"/>
-      <c r="Y19" s="51" t="e">
+        <v>-0.73029674334022143</v>
+      </c>
+      <c r="X19" s="34"/>
+      <c r="Y19" s="47" t="e">
         <f>(X19-AVERAGE($D19,$I19,$N19,$S19,$X19))/STDEV($D19,$I19,$N19,$S19,$X19)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z19" s="43">
+      <c r="Z19" s="39">
         <f>100*AA19/$C19</f>
         <v>0</v>
       </c>
-      <c r="AA19" s="44"/>
+      <c r="AA19" s="40"/>
       <c r="AB19" s="11">
         <f>(Z19-AVERAGE($F19,$K19,$P19,$U19,$Z19))/STDEV($F19,$K19,$P19,$U19,$Z19)</f>
-        <v>-0.44721359549995798</v>
+        <v>-0.73029674334022143</v>
       </c>
     </row>
     <row r="20" spans="1:28" ht="21" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="60">
+      <c r="B20" s="56">
         <f>AVERAGE(B16:B19)</f>
-        <v>0.83865482416764392</v>
+        <v>2.3432967525492594</v>
       </c>
       <c r="C20" s="5">
         <f>AVERAGE(C16:C19)</f>
         <v>394555.75</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="66">
         <f>AVERAGE(D16:D19)</f>
-        <v>1.7075E-2</v>
+        <v>2.0125000000000001E-2</v>
       </c>
       <c r="E20" s="13" t="e">
-        <f t="shared" ref="E20:AB20" si="14">AVERAGE(E16:E19)</f>
+        <f t="shared" ref="E20:AB20" si="13">AVERAGE(E16:E19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F20" s="13">
-        <f t="shared" si="14"/>
-        <v>4.1932741208382209</v>
+        <f t="shared" si="13"/>
+        <v>5.8588166441834577</v>
       </c>
       <c r="G20" s="14">
-        <f t="shared" si="14"/>
-        <v>17912.5</v>
+        <f t="shared" si="13"/>
+        <v>22936</v>
       </c>
       <c r="H20" s="13">
-        <f t="shared" si="14"/>
-        <v>1.7888543819998319</v>
-      </c>
-      <c r="I20" s="13" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
+        <v>1.0963343017322345</v>
+      </c>
+      <c r="I20" s="66">
+        <f t="shared" si="13"/>
+        <v>2.0125000000000001E-2</v>
+      </c>
+      <c r="J20" s="13" t="e">
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J20" s="13" t="e">
-        <f t="shared" si="14"/>
+      <c r="K20" s="13">
+        <f t="shared" si="13"/>
+        <v>5.8576671185628388</v>
+      </c>
+      <c r="L20" s="14">
+        <f>AVERAGE(L16:L19)</f>
+        <v>22937.25</v>
+      </c>
+      <c r="M20" s="13">
+        <f t="shared" si="13"/>
+        <v>1.0945206250763935</v>
+      </c>
+      <c r="N20" s="48" t="e">
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K20" s="13">
-        <f t="shared" si="14"/>
+      <c r="O20" s="49" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P20" s="48">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="L20" s="14" t="e">
-        <f t="shared" si="14"/>
+      <c r="Q20" s="14" t="e">
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M20" s="13">
-        <f t="shared" si="14"/>
-        <v>-0.44721359549995798</v>
-      </c>
-      <c r="N20" s="52" t="e">
-        <f t="shared" si="14"/>
+      <c r="R20" s="49">
+        <f>AVERAGE(R16:R19)</f>
+        <v>-0.73028497560287597</v>
+      </c>
+      <c r="S20" s="13" t="e">
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O20" s="53" t="e">
-        <f t="shared" si="14"/>
+      <c r="T20" s="13" t="e">
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P20" s="52">
-        <f t="shared" si="14"/>
+      <c r="U20" s="13">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="Q20" s="14" t="e">
-        <f t="shared" si="14"/>
+      <c r="V20" s="14" t="e">
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R20" s="53">
-        <f>AVERAGE(R16:R19)</f>
-        <v>-0.44721359549995798</v>
-      </c>
-      <c r="S20" s="13" t="e">
-        <f t="shared" si="14"/>
+      <c r="W20" s="13">
+        <f t="shared" si="13"/>
+        <v>-0.73028497560287597</v>
+      </c>
+      <c r="X20" s="13" t="e">
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T20" s="13" t="e">
-        <f t="shared" si="14"/>
+      <c r="Y20" s="13" t="e">
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="U20" s="13">
-        <f t="shared" si="14"/>
+      <c r="Z20" s="13">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="V20" s="14" t="e">
-        <f t="shared" si="14"/>
+      <c r="AA20" s="14" t="e">
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="W20" s="13">
-        <f t="shared" si="14"/>
-        <v>-0.44721359549995798</v>
-      </c>
-      <c r="X20" s="13" t="e">
-        <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y20" s="13" t="e">
-        <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z20" s="13">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AA20" s="14" t="e">
-        <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="AB20" s="13">
-        <f t="shared" si="14"/>
-        <v>-0.44721359549995798</v>
+        <f t="shared" si="13"/>
+        <v>-0.73028497560287597</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs - tested itkgray edit / allows to skip it
-add the option to skip itkGray step in pipeline
-add more step description
-updated documentation with itkgray edit tests
</commit_message>
<xml_diff>
--- a/Documentation/results all tests.xlsx
+++ b/Documentation/results all tests.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23840" windowHeight="15600" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24680" windowHeight="15600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="varying ref for MC" sheetId="1" r:id="rId1"/>
     <sheet name="varying nifti header fix" sheetId="4" r:id="rId2"/>
     <sheet name="varying class edit" sheetId="5" r:id="rId3"/>
+    <sheet name="slice timing correction" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="47">
   <si>
     <t>a)</t>
   </si>
@@ -147,6 +148,21 @@
   </si>
   <si>
     <t>Edited or unedited class file (with itkGray)</t>
+  </si>
+  <si>
+    <t>nb of handles edited</t>
+  </si>
+  <si>
+    <t>KM79 / new_pipeline_JAS_6_edited</t>
+  </si>
+  <si>
+    <t>LYY65 / new_pipeline_JAS_6_unedited</t>
+  </si>
+  <si>
+    <t>DC95 / new_pipeline_JAS_6_unedited</t>
+  </si>
+  <si>
+    <t>MV40 new_pipeline_JAS_3A_retest_full new_pipeline_JAS_3A_unedited</t>
   </si>
 </sst>
 </file>
@@ -349,7 +365,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -453,8 +469,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -619,6 +647,19 @@
     <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -643,17 +684,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="115">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -705,6 +737,12 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -756,6 +794,12 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1132,99 +1176,99 @@
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
       <c r="F1" s="50"/>
-      <c r="H1" s="60" t="s">
+      <c r="H1" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
     </row>
     <row r="2" spans="1:28" ht="78" customHeight="1">
       <c r="E2" s="50"/>
       <c r="F2" s="50"/>
       <c r="G2" s="50"/>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60" t="s">
+      <c r="I2" s="65"/>
+      <c r="J2" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="67"/>
-      <c r="L2" s="64" t="s">
+      <c r="K2" s="72"/>
+      <c r="L2" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="60"/>
+      <c r="M2" s="65"/>
     </row>
     <row r="3" spans="1:28" ht="21" customHeight="1">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="65">
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="70">
         <v>2.0125000000000001E-2</v>
       </c>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66">
+      <c r="I3" s="70"/>
+      <c r="J3" s="71">
         <v>5.8588166441834577</v>
       </c>
-      <c r="K3" s="66"/>
-      <c r="L3" s="60">
+      <c r="K3" s="71"/>
+      <c r="L3" s="65">
         <v>22936</v>
       </c>
-      <c r="M3" s="60"/>
+      <c r="M3" s="65"/>
     </row>
     <row r="4" spans="1:28" ht="15" customHeight="1">
-      <c r="A4" s="60"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
     </row>
     <row r="5" spans="1:28" ht="20" customHeight="1">
-      <c r="A5" s="60"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
     </row>
     <row r="6" spans="1:28" ht="20" customHeight="1">
-      <c r="A6" s="60"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
     </row>
     <row r="7" spans="1:28">
       <c r="A7" s="52" t="s">
@@ -1260,22 +1304,22 @@
       <c r="C13" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="63"/>
-      <c r="L13" s="63"/>
-      <c r="M13" s="63"/>
-      <c r="N13" s="63"/>
-      <c r="O13" s="63"/>
-      <c r="P13" s="63"/>
-      <c r="Q13" s="63"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="68"/>
+      <c r="P13" s="68"/>
+      <c r="Q13" s="68"/>
       <c r="R13" s="55"/>
       <c r="S13" s="55"/>
       <c r="T13" s="55"/>
@@ -1289,10 +1333,10 @@
       <c r="AB13" s="55"/>
     </row>
     <row r="14" spans="1:28" ht="31" customHeight="1" thickBot="1">
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="62"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="6" t="s">
         <v>0</v>
       </c>
@@ -1949,8 +1993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C16" sqref="C15:C16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1992,93 +2036,93 @@
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
       <c r="F1" s="50"/>
-      <c r="H1" s="60" t="s">
+      <c r="H1" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
     </row>
     <row r="2" spans="1:28" ht="20">
       <c r="E2" s="50"/>
       <c r="F2" s="50"/>
       <c r="G2" s="50"/>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60" t="s">
+      <c r="I2" s="65"/>
+      <c r="J2" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="67"/>
-      <c r="L2" s="64" t="s">
+      <c r="K2" s="72"/>
+      <c r="L2" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="60"/>
+      <c r="M2" s="65"/>
     </row>
     <row r="3" spans="1:28" ht="21" customHeight="1">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
     </row>
     <row r="4" spans="1:28" ht="15" customHeight="1">
-      <c r="A4" s="60"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
     </row>
     <row r="5" spans="1:28" ht="20" customHeight="1">
-      <c r="A5" s="60"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
     </row>
     <row r="6" spans="1:28" ht="20" customHeight="1">
-      <c r="A6" s="60"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
     </row>
     <row r="7" spans="1:28">
       <c r="A7" s="52" t="s">
@@ -2108,22 +2152,22 @@
       <c r="C13" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="63"/>
-      <c r="L13" s="63"/>
-      <c r="M13" s="63"/>
-      <c r="N13" s="63"/>
-      <c r="O13" s="63"/>
-      <c r="P13" s="63"/>
-      <c r="Q13" s="63"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="68"/>
+      <c r="P13" s="68"/>
+      <c r="Q13" s="68"/>
       <c r="R13" s="55"/>
       <c r="S13" s="55"/>
       <c r="T13" s="55"/>
@@ -2137,10 +2181,10 @@
       <c r="AB13" s="55"/>
     </row>
     <row r="14" spans="1:28" ht="31" customHeight="1" thickBot="1">
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="62"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="6" t="s">
         <v>0</v>
       </c>
@@ -2747,48 +2791,52 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="52" customFormat="1">
+    <row r="1" spans="1:17" s="52" customFormat="1">
       <c r="A1" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="K1" s="52" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" thickBot="1">
+    <row r="2" spans="1:17" ht="15" customHeight="1" thickBot="1">
       <c r="C2" t="s">
         <v>37</v>
       </c>
       <c r="F2" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="60" t="s">
+      <c r="K2" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-    </row>
-    <row r="3" spans="1:16" ht="76" thickBot="1">
-      <c r="B3" s="69" t="s">
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+    </row>
+    <row r="3" spans="1:17" ht="76" thickBot="1">
+      <c r="B3" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="60" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="10" t="s">
@@ -2797,7 +2845,7 @@
       <c r="E3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="68" t="s">
+      <c r="F3" s="60" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="10" t="s">
@@ -2806,68 +2854,218 @@
       <c r="H3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="70" t="s">
+      <c r="I3" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-    </row>
-    <row r="4" spans="1:16" ht="20">
-      <c r="A4" t="s">
-        <v>5</v>
+      <c r="J3" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+    </row>
+    <row r="4" spans="1:17" ht="62" thickBot="1">
+      <c r="A4" s="63" t="s">
+        <v>46</v>
       </c>
       <c r="B4" s="2">
         <v>349890</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="64">
         <v>1.84E-2</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="64">
         <f>100*E4/$B4</f>
         <v>5.6700677355740376</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="64">
         <v>19839</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="64">
         <v>1.84E-2</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="64">
         <f>100*H4/$B4</f>
         <v>5.6700677355740376</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="64">
         <v>19839</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="64">
         <f>C4-F4</f>
         <v>0</v>
       </c>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="60"/>
-      <c r="P5" s="60"/>
+      <c r="J4" s="64">
+        <v>1</v>
+      </c>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="65"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="65"/>
+    </row>
+    <row r="5" spans="1:17" ht="61" thickBot="1">
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="2">
+        <v>406142</v>
+      </c>
+      <c r="C5" s="64">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="D5" s="64">
+        <f t="shared" ref="D5:D7" si="0">100*E5/$B5</f>
+        <v>5.6642750565073303</v>
+      </c>
+      <c r="E5" s="64">
+        <v>23005</v>
+      </c>
+      <c r="F5" s="64">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="G5" s="64">
+        <f>100*H5/$B5</f>
+        <v>5.6642750565073303</v>
+      </c>
+      <c r="H5" s="64">
+        <v>23005</v>
+      </c>
+      <c r="I5" s="64">
+        <f t="shared" ref="I5:I7" si="1">C5-F5</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="64">
+        <v>3</v>
+      </c>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="65"/>
+    </row>
+    <row r="6" spans="1:17" ht="61" thickBot="1">
+      <c r="A6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="1">
+        <v>377743</v>
+      </c>
+      <c r="C6" s="64">
+        <v>2.46E-2</v>
+      </c>
+      <c r="D6" s="64">
+        <f t="shared" si="0"/>
+        <v>7.3192620379464346</v>
+      </c>
+      <c r="E6" s="64">
+        <v>27648</v>
+      </c>
+      <c r="F6" s="64">
+        <v>2.46E-2</v>
+      </c>
+      <c r="G6" s="64">
+        <f t="shared" ref="G6:G7" si="2">100*H6/$B6</f>
+        <v>7.318467847187109</v>
+      </c>
+      <c r="H6" s="64">
+        <v>27645</v>
+      </c>
+      <c r="I6" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="64">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="61" thickBot="1">
+      <c r="A7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="1">
+        <v>444448</v>
+      </c>
+      <c r="C7" s="64">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="D7" s="64">
+        <f t="shared" si="0"/>
+        <v>4.7816617467060265</v>
+      </c>
+      <c r="E7" s="64">
+        <v>21252</v>
+      </c>
+      <c r="F7" s="64">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="G7" s="64">
+        <f t="shared" si="2"/>
+        <v>4.7816617467060265</v>
+      </c>
+      <c r="H7" s="64">
+        <v>21252</v>
+      </c>
+      <c r="I7" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="64">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="21" thickBot="1">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5">
+        <f>AVERAGE(B4:B7)</f>
+        <v>394555.75</v>
+      </c>
+      <c r="C8" s="64">
+        <f>AVERAGE(C4:C7)</f>
+        <v>2.0125000000000001E-2</v>
+      </c>
+      <c r="D8" s="64">
+        <f>AVERAGE(D4:D7)</f>
+        <v>5.8588166441834577</v>
+      </c>
+      <c r="E8" s="64">
+        <f t="shared" ref="E8:J8" si="3">AVERAGE(E4:E7)</f>
+        <v>22936</v>
+      </c>
+      <c r="F8" s="64">
+        <f t="shared" si="3"/>
+        <v>2.0125000000000001E-2</v>
+      </c>
+      <c r="G8" s="64">
+        <f t="shared" si="3"/>
+        <v>5.8586180964936254</v>
+      </c>
+      <c r="H8" s="64">
+        <f>AVERAGE(H4:H7)</f>
+        <v>22935.25</v>
+      </c>
+      <c r="I8" s="64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="64">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="J2:P5"/>
+    <mergeCell ref="K2:Q5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2877,4 +3075,21 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>